<commit_message>
Created the form tempelate
</commit_message>
<xml_diff>
--- a/docs/documents/status/Project Progress.xlsx
+++ b/docs/documents/status/Project Progress.xlsx
@@ -5,37 +5,28 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Documention\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sampathproducts\docs\documents\status\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E785EBD-E38A-490D-B5C7-DBBBA74979B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D4243F-5575-44A0-9C7A-2792D669270D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{4BBF5CEB-B3BB-458A-B42B-679A065AE060}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Module creation" sheetId="1" r:id="rId1"/>
+    <sheet name="Projet logs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>No</t>
   </si>
@@ -143,6 +134,48 @@
   </si>
   <si>
     <t>Customer Order Report</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Created the Table View UI tempelate</t>
+  </si>
+  <si>
+    <t>23/10/2023</t>
+  </si>
+  <si>
+    <t>Decided the project topic</t>
+  </si>
+  <si>
+    <t>28/10/2023</t>
+  </si>
+  <si>
+    <t>Gathering Requirements</t>
+  </si>
+  <si>
+    <t>30/10/2023</t>
+  </si>
+  <si>
+    <t>Defining the scope and created the scope Documents</t>
+  </si>
+  <si>
+    <t>Module Identification</t>
+  </si>
+  <si>
+    <t>Create the module based attibute list (er-word)</t>
+  </si>
+  <si>
+    <t>Designing the ER -Diagram</t>
+  </si>
+  <si>
+    <t>15/11/2023</t>
+  </si>
+  <si>
+    <t>Wireframe drawing started</t>
   </si>
 </sst>
 </file>
@@ -222,16 +255,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -549,7 +594,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A38C62ED-9DA5-4DDD-8AAE-F404D5599198}">
   <dimension ref="B2:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -603,7 +648,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="4"/>
+      <c r="I3" s="3"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
@@ -619,7 +664,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="4"/>
+      <c r="I4" s="3"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
@@ -715,7 +760,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="4"/>
+      <c r="I10" s="3"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
@@ -731,7 +776,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="4"/>
+      <c r="I11" s="3"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
@@ -896,42 +941,42 @@
       <c r="K21" s="2"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <v>20</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="3">
+      <c r="B23" s="2">
         <v>21</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="3">
+      <c r="B24" s="2">
         <v>22</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D24" s="2"/>
@@ -944,18 +989,18 @@
       <c r="K24" s="2"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
@@ -967,9 +1012,9 @@
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
@@ -983,9 +1028,9 @@
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
@@ -999,9 +1044,9 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
     </row>
@@ -1015,9 +1060,9 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
@@ -1028,4 +1073,95 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87EF18B3-1218-4FA4-94C1-A4F1282F1E4B}">
+  <dimension ref="C3:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="18.7109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="59.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="8">
+        <v>44968</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="8">
+        <v>45057</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="8">
+        <v>45210</v>
+      </c>
+      <c r="D9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="8">
+        <v>44938</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Proposal Documentation - 2
</commit_message>
<xml_diff>
--- a/docs/documents/status/Project Progress.xlsx
+++ b/docs/documents/status/Project Progress.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sampathproducts\docs\documents\status\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D4243F-5575-44A0-9C7A-2792D669270D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{59C7A2D6-E0C0-4180-954E-5D396A6D96A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{4BBF5CEB-B3BB-458A-B42B-679A065AE060}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Projet logs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -262,9 +263,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -277,6 +275,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -592,21 +593,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A38C62ED-9DA5-4DDD-8AAE-F404D5599198}">
-  <dimension ref="B2:K29"/>
+  <dimension ref="B2:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="22.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" customWidth="1"/>
+    <col min="5" max="5" width="8" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" customWidth="1"/>
+    <col min="7" max="8" width="8.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -616,27 +621,26 @@
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="F2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="2">
         <v>1</v>
       </c>
@@ -647,12 +651,11 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>2</v>
       </c>
@@ -663,12 +666,11 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>3</v>
       </c>
@@ -682,9 +684,8 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>4</v>
       </c>
@@ -698,9 +699,8 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>5</v>
       </c>
@@ -714,9 +714,8 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>6</v>
       </c>
@@ -730,9 +729,8 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>7</v>
       </c>
@@ -746,9 +744,8 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>8</v>
       </c>
@@ -759,12 +756,11 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>9</v>
       </c>
@@ -775,12 +771,11 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>10</v>
       </c>
@@ -794,9 +789,8 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>11</v>
       </c>
@@ -810,9 +804,8 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <v>12</v>
       </c>
@@ -826,9 +819,8 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <v>13</v>
       </c>
@@ -842,9 +834,8 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
         <v>14</v>
       </c>
@@ -858,9 +849,8 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
         <v>15</v>
       </c>
@@ -874,9 +864,8 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
         <v>16</v>
       </c>
@@ -890,9 +879,8 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
         <v>17</v>
       </c>
@@ -906,9 +894,8 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
         <v>18</v>
       </c>
@@ -922,9 +909,8 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
         <v>19</v>
       </c>
@@ -938,9 +924,8 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
         <v>20</v>
       </c>
@@ -949,14 +934,13 @@
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+      <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
+      <c r="I22" s="2"/>
       <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
         <v>21</v>
       </c>
@@ -965,14 +949,13 @@
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+      <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
+      <c r="I23" s="2"/>
       <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
         <v>22</v>
       </c>
@@ -986,23 +969,21 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="4" t="s">
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
         <v>23</v>
       </c>
@@ -1011,14 +992,13 @@
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
+      <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
+      <c r="I26" s="2"/>
       <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="2">
         <v>24</v>
       </c>
@@ -1027,14 +1007,13 @@
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
+      <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
+      <c r="I27" s="2"/>
       <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
         <v>25</v>
       </c>
@@ -1043,14 +1022,13 @@
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+      <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
+      <c r="I28" s="2"/>
       <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="2">
         <v>26</v>
       </c>
@@ -1059,16 +1037,15 @@
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
+      <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
+      <c r="I29" s="2"/>
       <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B25:K25"/>
+    <mergeCell ref="B25:J25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1085,20 +1062,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="4" customWidth="1"/>
     <col min="4" max="4" width="59.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>39</v>
       </c>
       <c r="D4" t="s">
@@ -1106,7 +1083,7 @@
       </c>
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>41</v>
       </c>
       <c r="D5" t="s">
@@ -1114,7 +1091,7 @@
       </c>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>43</v>
       </c>
       <c r="D6" t="s">
@@ -1122,7 +1099,7 @@
       </c>
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="8">
+      <c r="C7" s="7">
         <v>44968</v>
       </c>
       <c r="D7" t="s">
@@ -1130,7 +1107,7 @@
       </c>
     </row>
     <row r="8" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="8">
+      <c r="C8" s="7">
         <v>45057</v>
       </c>
       <c r="D8" t="s">
@@ -1138,7 +1115,7 @@
       </c>
     </row>
     <row r="9" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C9" s="8">
+      <c r="C9" s="7">
         <v>45210</v>
       </c>
       <c r="D9" t="s">
@@ -1146,7 +1123,7 @@
       </c>
     </row>
     <row r="10" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>48</v>
       </c>
       <c r="D10" t="s">
@@ -1154,10 +1131,10 @@
       </c>
     </row>
     <row r="11" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C11" s="8">
+      <c r="C11" s="7">
         <v>44938</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="8" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>